<commit_message>
add logic to track the two rectangular contours
</commit_message>
<xml_diff>
--- a/marking_scheme.xlsx
+++ b/marking_scheme.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nuran\MyWork\coding\repos\computer_vision\mcq_grader\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nuran\MyWork\coding\repos\Automated-MCQ-grading\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3033D9D-621F-476E-9E0D-DB6E2DC5E86E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF8E9A1-169B-4881-8109-CB1D4BD8E02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{206D7788-4370-4B66-97E2-80F46CED16D5}"/>
   </bookViews>
@@ -394,7 +394,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -412,7 +412,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -444,7 +444,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upgrade grader to grade 50 MCQs
</commit_message>
<xml_diff>
--- a/marking_scheme.xlsx
+++ b/marking_scheme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nuran\MyWork\coding\repos\Automated-MCQ-grading\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF8E9A1-169B-4881-8109-CB1D4BD8E02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F30A6AE-659C-41D9-A79D-A4E91A17B63A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{206D7788-4370-4B66-97E2-80F46CED16D5}"/>
   </bookViews>
@@ -391,15 +391,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60E7AF2B-F68C-4EE1-857C-35F5B19B247B}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -407,44 +407,710 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>2</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>4</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>3</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D53">
+        <f>COUNTIF(B2:B51,"=0")</f>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>